<commit_message>
add non-linear logistic regression
</commit_message>
<xml_diff>
--- a/Data/forged-bank-notes.xlsx
+++ b/Data/forged-bank-notes.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="640" yWindow="1180" windowWidth="24960" windowHeight="14820" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="760" yWindow="640" windowWidth="24960" windowHeight="14820" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
@@ -528,8 +528,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:E1373"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -23884,7 +23884,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:A18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>

</xml_diff>